<commit_message>
Located the gantt chart
</commit_message>
<xml_diff>
--- a/NoGracias/ScrumDogs/Logs.xlsx
+++ b/NoGracias/ScrumDogs/Logs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
   <si>
     <t>Task</t>
   </si>
@@ -227,15 +227,26 @@
   </si>
   <si>
     <t>Take the Card table design and begin population of the User Interface</t>
+  </si>
+  <si>
+    <t>Full Design on png file in the folder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -268,11 +279,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1251,16 +1263,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1545,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1668,12 +1680,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:5" ht="46.2" x14ac:dyDescent="0.85">
+      <c r="E21" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1856,7 +1874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>

</xml_diff>